<commit_message>
thêm cột Mã CQT cấp cho xuất khẩu excel
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/HoaDonDienTu/BANG_KE_HOA_DON_DIEN_TU.xlsx
+++ b/API/wwwroot/docs/HoaDonDienTu/BANG_KE_HOA_DON_DIEN_TU.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIT\bill-back-end\API\wwwroot\docs\HoaDonDienTu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pmbk\bills\bill-back-end\API\wwwroot\docs\HoaDonDienTu\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>BẢNG KÊ HÓA ĐƠN ĐIỆN TỬ</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>Người lập</t>
+  </si>
+  <si>
+    <t>Mã CQT cấp</t>
   </si>
 </sst>
 </file>
@@ -247,12 +250,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
     </xf>
@@ -260,6 +257,12 @@
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma 2" xfId="3"/>
@@ -578,101 +581,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="21.44140625" customWidth="1"/>
-    <col min="7" max="7" width="39" customWidth="1"/>
-    <col min="8" max="8" width="23.6640625" customWidth="1"/>
-    <col min="9" max="10" width="28.5546875" customWidth="1"/>
-    <col min="11" max="11" width="29.5546875" customWidth="1"/>
-    <col min="12" max="12" width="29.6640625" customWidth="1"/>
-    <col min="13" max="13" width="26.33203125" customWidth="1"/>
-    <col min="14" max="14" width="19.5546875" customWidth="1"/>
-    <col min="15" max="15" width="22.109375" customWidth="1"/>
-    <col min="16" max="16" width="24" customWidth="1"/>
-    <col min="17" max="17" width="25.88671875" customWidth="1"/>
-    <col min="18" max="18" width="28.6640625" customWidth="1"/>
-    <col min="19" max="19" width="24.109375" customWidth="1"/>
-    <col min="20" max="20" width="29.33203125" customWidth="1"/>
-    <col min="21" max="21" width="30.6640625" customWidth="1"/>
-    <col min="22" max="22" width="30.33203125" customWidth="1"/>
-    <col min="23" max="23" width="37.33203125" customWidth="1"/>
-    <col min="24" max="24" width="21.33203125" customWidth="1"/>
-    <col min="25" max="25" width="20.88671875" customWidth="1"/>
-    <col min="26" max="26" width="18.5546875" customWidth="1"/>
+    <col min="3" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="27" customWidth="1"/>
+    <col min="6" max="6" width="25" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" customWidth="1"/>
+    <col min="8" max="8" width="39" customWidth="1"/>
+    <col min="9" max="9" width="23.6640625" customWidth="1"/>
+    <col min="10" max="11" width="28.5546875" customWidth="1"/>
+    <col min="12" max="12" width="29.5546875" customWidth="1"/>
+    <col min="13" max="13" width="29.6640625" customWidth="1"/>
+    <col min="14" max="14" width="26.33203125" customWidth="1"/>
+    <col min="15" max="15" width="19.5546875" customWidth="1"/>
+    <col min="16" max="16" width="22.109375" customWidth="1"/>
+    <col min="17" max="17" width="24" customWidth="1"/>
+    <col min="18" max="18" width="25.88671875" customWidth="1"/>
+    <col min="19" max="19" width="28.6640625" customWidth="1"/>
+    <col min="20" max="20" width="24.109375" customWidth="1"/>
+    <col min="21" max="21" width="29.33203125" customWidth="1"/>
+    <col min="22" max="22" width="30.6640625" customWidth="1"/>
+    <col min="23" max="23" width="30.33203125" customWidth="1"/>
+    <col min="24" max="24" width="37.33203125" customWidth="1"/>
+    <col min="25" max="25" width="21.33203125" customWidth="1"/>
+    <col min="26" max="26" width="20.88671875" customWidth="1"/>
+    <col min="27" max="27" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:27" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+      <c r="AA2" s="9"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="1"/>
@@ -699,8 +704,9 @@
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -711,107 +717,111 @@
         <v>4</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AA4" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
+    <row r="5" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:Z1"/>
-    <mergeCell ref="A2:Z2"/>
+    <mergeCell ref="A1:AA1"/>
+    <mergeCell ref="A2:AA2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>